<commit_message>
novo método de análise de in/out implementado, e algumas outras mudanças pontuais
</commit_message>
<xml_diff>
--- a/data/input/SR_Smoothing_Measured_ML.xlsx
+++ b/data/input/SR_Smoothing_Measured_ML.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.neto\Desktop\Script-Automatizacao-SA\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.neto\Desktop\Script-Automatizacao-SA\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E225C1-021F-4254-B06F-89371160D5F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA76F405-DE95-4614-AC0C-62C0C9A57AF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="1815" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
   <si>
     <t>S18-B01-C01</t>
   </si>
@@ -234,24 +234,6 @@
   </si>
   <si>
     <t>S09-B07-C04</t>
-  </si>
-  <si>
-    <t>S14-B11-C03-B1*</t>
-  </si>
-  <si>
-    <t>S14-B11-C04-B1MR*</t>
-  </si>
-  <si>
-    <t>S14-B11-C09*</t>
-  </si>
-  <si>
-    <t>S14-B11-C10*</t>
-  </si>
-  <si>
-    <t>S14-B11-C11*</t>
-  </si>
-  <si>
-    <t>S14-B11-C12*</t>
   </si>
   <si>
     <t>S05-B07-C03</t>
@@ -1010,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D220"/>
+  <dimension ref="A1:D214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,3085 +1005,3004 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="B1">
-        <v>80934.330642000001</v>
+        <v>-45065.781927999997</v>
       </c>
       <c r="C1">
-        <v>-14436.102134999999</v>
+        <v>-68710.522498999999</v>
       </c>
       <c r="D1">
-        <v>1628.5660640000001</v>
+        <v>1628.5256119999999</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>204</v>
       </c>
       <c r="B2">
-        <v>81232.481304000001</v>
+        <v>-45223.625820000001</v>
       </c>
       <c r="C2">
-        <v>-14504.922973999999</v>
+        <v>-68972.688909000004</v>
       </c>
       <c r="D2">
-        <v>1628.6097130000001</v>
+        <v>1628.5243049999999</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>205</v>
       </c>
       <c r="B3">
-        <v>81030.198696000007</v>
+        <v>-45995.459014</v>
       </c>
       <c r="C3">
-        <v>-15381.054975999999</v>
+        <v>-68508.894602</v>
       </c>
       <c r="D3">
-        <v>1628.6197770000001</v>
+        <v>1628.5006980000001</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>206</v>
       </c>
       <c r="B4">
-        <v>80732.026761999994</v>
+        <v>-45837.370858000002</v>
       </c>
       <c r="C4">
-        <v>-15312.466528999999</v>
+        <v>-68246.860858</v>
       </c>
       <c r="D4">
-        <v>1628.6192980000001</v>
+        <v>1628.4827760000001</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="B5">
-        <v>79274.066523000001</v>
+        <v>-50031.325087999998</v>
       </c>
       <c r="C5">
-        <v>-21628.189342000001</v>
+        <v>-65782.288986</v>
       </c>
       <c r="D5">
-        <v>1628.6438430000001</v>
+        <v>1628.5078619999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="B6">
-        <v>79572.198252000002</v>
+        <v>-50311.882017999997</v>
       </c>
       <c r="C6">
-        <v>-21697.032078</v>
+        <v>-65579.884220000007</v>
       </c>
       <c r="D6">
-        <v>1628.6916859999999</v>
+        <v>1628.466093</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B7">
-        <v>79369.494451000006</v>
+        <v>-49683.837793999999</v>
       </c>
       <c r="C7">
-        <v>-22574.335514999999</v>
+        <v>-66033.140010999996</v>
       </c>
       <c r="D7">
-        <v>1628.678774</v>
+        <v>1628.4670470000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="B8">
-        <v>79071.456109999999</v>
+        <v>-49995.558626999999</v>
       </c>
       <c r="C8">
-        <v>-22505.008741000001</v>
+        <v>-65441.839439000003</v>
       </c>
       <c r="D8">
-        <v>1628.6178849999999</v>
+        <v>1628.3685640000001</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="B9">
-        <v>66971.154806999999</v>
+        <v>-50658.465701000001</v>
       </c>
       <c r="C9">
-        <v>-47866.098901999998</v>
+        <v>-65329.963500999998</v>
       </c>
       <c r="D9">
-        <v>1628.799704</v>
+        <v>1628.416545</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="B10">
-        <v>67225.510158999998</v>
+        <v>-50897.876967999997</v>
       </c>
       <c r="C10">
-        <v>-48036.269286000002</v>
+        <v>-64851.905810999997</v>
       </c>
       <c r="D10">
-        <v>1628.8840970000001</v>
+        <v>1628.379619</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="B11">
-        <v>66296.619153000007</v>
+        <v>-51085.779866999997</v>
       </c>
       <c r="C11">
-        <v>-49426.104474</v>
+        <v>-65093.474029999998</v>
       </c>
       <c r="D11">
-        <v>1628.886718</v>
+        <v>1628.416444</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="B12">
-        <v>66042.137417000005</v>
+        <v>-52145.941112</v>
       </c>
       <c r="C12">
-        <v>-49256.099554</v>
+        <v>-64269.652409000002</v>
       </c>
       <c r="D12">
-        <v>1628.81059</v>
+        <v>1628.482393</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="B13">
-        <v>59975.624873000001</v>
+        <v>-51958.052589999999</v>
       </c>
       <c r="C13">
-        <v>-56485.835679000003</v>
+        <v>-64028.130054000001</v>
       </c>
       <c r="D13">
-        <v>1628.6832649999999</v>
+        <v>1628.3734019999999</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
       <c r="B14">
-        <v>60187.260206999999</v>
+        <v>-52634.707397999999</v>
       </c>
       <c r="C14">
-        <v>-56706.876279999997</v>
+        <v>-63427.906902000002</v>
       </c>
       <c r="D14">
-        <v>1628.7549819999999</v>
+        <v>1751.4253920000001</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
       <c r="B15">
-        <v>58980.168005</v>
+        <v>-52849.422150999999</v>
       </c>
       <c r="C15">
-        <v>-57862.651485000002</v>
+        <v>-63683.749931999999</v>
       </c>
       <c r="D15">
-        <v>1628.6924879999999</v>
+        <v>1751.404198</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="B16">
-        <v>58768.585911000002</v>
+        <v>-53538.076654999997</v>
       </c>
       <c r="C16">
-        <v>-57641.555157000003</v>
+        <v>-63106.050764</v>
       </c>
       <c r="D16">
-        <v>1628.6476580000001</v>
+        <v>1751.355157</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>126</v>
       </c>
       <c r="B17">
-        <v>57703.702570000001</v>
+        <v>-53323.315569999999</v>
       </c>
       <c r="C17">
-        <v>-59037.973052000001</v>
+        <v>-62850.201738000003</v>
       </c>
       <c r="D17">
-        <v>1628.7402850000001</v>
+        <v>1751.3973960000001</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B18">
-        <v>57502.911726999999</v>
+        <v>-54032.775780000004</v>
       </c>
       <c r="C18">
-        <v>-58807.101329999998</v>
+        <v>-62287.188003000003</v>
       </c>
       <c r="D18">
-        <v>1628.5749940000001</v>
+        <v>1628.4069979999999</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B19">
-        <v>57184.696201999999</v>
+        <v>-54238.199625000001</v>
       </c>
       <c r="C19">
-        <v>-59083.803965999999</v>
+        <v>-62514.033709000003</v>
       </c>
       <c r="D19">
-        <v>1628.586728</v>
+        <v>1628.3379640000001</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B20">
-        <v>57385.526585</v>
+        <v>-55233.886749999998</v>
       </c>
       <c r="C20">
-        <v>-59314.733445999998</v>
+        <v>-61613.001640000002</v>
       </c>
       <c r="D20">
-        <v>1628.7335860000001</v>
+        <v>1628.348107</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B21">
-        <v>58197.202144000003</v>
+        <v>-55028.476653999998</v>
       </c>
       <c r="C21">
-        <v>-58487.781667000003</v>
+        <v>-61386.176392000001</v>
       </c>
       <c r="D21">
-        <v>1628.795656</v>
+        <v>1628.322009</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B22">
-        <v>58149.543564</v>
+        <v>-55847.149252000003</v>
       </c>
       <c r="C22">
-        <v>-58531.026583999999</v>
+        <v>-60935.409109</v>
       </c>
       <c r="D22">
-        <v>1628.831459</v>
+        <v>1628.4040359999999</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B23">
-        <v>47589.051968</v>
+        <v>-56095.075647999998</v>
       </c>
       <c r="C23">
-        <v>-67253.396653000003</v>
+        <v>-60694.381052999997</v>
       </c>
       <c r="D23">
-        <v>1628.3378600000001</v>
+        <v>1628.3783129999999</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B24">
-        <v>48901.755111999999</v>
+        <v>-55690.239810999999</v>
       </c>
       <c r="C24">
-        <v>-66218.760722999999</v>
+        <v>-61094.806146000003</v>
       </c>
       <c r="D24">
-        <v>1628.3589380000001</v>
+        <v>1628.3654260000001</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B25">
-        <v>49091.544134999996</v>
+        <v>-55772.497629999998</v>
       </c>
       <c r="C25">
-        <v>-66458.810536999998</v>
+        <v>-60593.736886999999</v>
       </c>
       <c r="D25">
-        <v>1628.4045590000001</v>
+        <v>1628.329232</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B26">
-        <v>47778.567331999999</v>
+        <v>-56253.752135000002</v>
       </c>
       <c r="C26">
-        <v>-67493.689155999993</v>
+        <v>-60547.002614999998</v>
       </c>
       <c r="D26">
-        <v>1628.384898</v>
+        <v>1628.3644730000001</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="B27">
-        <v>44057.660012</v>
+        <v>-69659.704652999993</v>
       </c>
       <c r="C27">
-        <v>-69660.147303000005</v>
+        <v>-44058.14273</v>
       </c>
       <c r="D27">
-        <v>1751.219542</v>
+        <v>1751.102801</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="B28">
-        <v>44234.664687999997</v>
+        <v>-69942.920217000006</v>
       </c>
       <c r="C28">
-        <v>-69943.440128000002</v>
+        <v>-44235.105387000003</v>
       </c>
       <c r="D28">
-        <v>1751.2733020000001</v>
+        <v>1751.118068</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="B29">
-        <v>43472.317158999998</v>
+        <v>-70419.250453000001</v>
       </c>
       <c r="C29">
-        <v>-70419.774533000003</v>
+        <v>-43472.800956999999</v>
       </c>
       <c r="D29">
-        <v>1751.2200660000001</v>
+        <v>1751.0736810000001</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B30">
-        <v>43295.335779000001</v>
+        <v>-70136.025787999999</v>
       </c>
       <c r="C30">
-        <v>-70136.483240000001</v>
+        <v>-43295.830716999997</v>
       </c>
       <c r="D30">
-        <v>1751.220343</v>
+        <v>1751.108835</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B31">
-        <v>81722.469494999998</v>
+        <v>-73608.967923000004</v>
       </c>
       <c r="C31">
-        <v>-10445.656853</v>
+        <v>-37276.056831000002</v>
       </c>
       <c r="D31">
-        <v>1628.573234</v>
+        <v>1628.306456</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="B32">
-        <v>82023.565625999996</v>
+        <v>-73635.643284000005</v>
       </c>
       <c r="C32">
-        <v>-10500.228024</v>
+        <v>-37217.039360000002</v>
       </c>
       <c r="D32">
-        <v>1628.601887</v>
+        <v>1628.2867759999999</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="B33">
-        <v>81726.368868999998</v>
+        <v>-73697.953878</v>
       </c>
       <c r="C33">
-        <v>-12145.191948</v>
+        <v>-36516.922000999999</v>
       </c>
       <c r="D33">
-        <v>1628.5951439999999</v>
+        <v>1628.1123170000001</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="B34">
-        <v>81425.250121999998</v>
+        <v>-73979.705845999997</v>
       </c>
       <c r="C34">
-        <v>-12090.67841</v>
+        <v>-36636.337194</v>
       </c>
       <c r="D34">
-        <v>1628.595687</v>
+        <v>1628.0378969999999</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="B35">
-        <v>-54032.775780000004</v>
+        <v>-74144.553941999999</v>
       </c>
       <c r="C35">
-        <v>-62287.188003000003</v>
+        <v>-36247.983831999998</v>
       </c>
       <c r="D35">
-        <v>1628.4069979999999</v>
+        <v>1628.072355</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="B36">
-        <v>-54238.199625000001</v>
+        <v>-73862.787184000001</v>
       </c>
       <c r="C36">
-        <v>-62514.033709000003</v>
+        <v>-36128.519823000002</v>
       </c>
       <c r="D36">
-        <v>1628.3379640000001</v>
+        <v>1628.0574509999999</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="B37">
-        <v>-55233.886749999998</v>
+        <v>-73962.438330999998</v>
       </c>
       <c r="C37">
-        <v>-61613.001640000002</v>
+        <v>-35893.836522999998</v>
       </c>
       <c r="D37">
-        <v>1628.348107</v>
+        <v>1628.112554</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="B38">
-        <v>-55028.476653999998</v>
+        <v>-74243.947371999995</v>
       </c>
       <c r="C38">
-        <v>-61386.176392000001</v>
+        <v>-36013.728722</v>
       </c>
       <c r="D38">
-        <v>1628.322009</v>
+        <v>1628.1087769999999</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="B39">
-        <v>-55690.239810999999</v>
+        <v>-74595.592084999997</v>
       </c>
       <c r="C39">
-        <v>-61094.806146000003</v>
+        <v>-35185.186755000002</v>
       </c>
       <c r="D39">
-        <v>1628.3654260000001</v>
+        <v>1628.0697849999999</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B40">
-        <v>-56253.752135000002</v>
+        <v>-74313.862127</v>
       </c>
       <c r="C40">
-        <v>-60547.002614999998</v>
+        <v>-35065.813776000003</v>
       </c>
       <c r="D40">
-        <v>1628.3644730000001</v>
+        <v>1628.1010679999999</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B41">
-        <v>-55772.497629999998</v>
+        <v>-76846.744223000002</v>
       </c>
       <c r="C41">
-        <v>-60593.736886999999</v>
+        <v>-29099.072069000002</v>
       </c>
       <c r="D41">
-        <v>1628.329232</v>
+        <v>1628.1673699999999</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="B42">
-        <v>-55847.149252000003</v>
+        <v>-77128.394448000006</v>
       </c>
       <c r="C42">
-        <v>-60935.409109</v>
+        <v>-29218.636632000002</v>
       </c>
       <c r="D42">
-        <v>1628.4040359999999</v>
+        <v>1628.0975370000001</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="B43">
-        <v>-56095.075647999998</v>
+        <v>-77479.950614999994</v>
       </c>
       <c r="C43">
-        <v>-60694.381052999997</v>
+        <v>-28390.141823000002</v>
       </c>
       <c r="D43">
-        <v>1628.3783129999999</v>
+        <v>1628.107591</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="B44">
-        <v>68710.525204999998</v>
+        <v>-77198.235436000003</v>
       </c>
       <c r="C44">
-        <v>-45066.885010999998</v>
+        <v>-28270.681487999998</v>
       </c>
       <c r="D44">
-        <v>1628.8684479999999</v>
+        <v>1628.182867</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B45">
-        <v>68972.805871999997</v>
+        <v>-77297.975154</v>
       </c>
       <c r="C45">
-        <v>-45224.516497999997</v>
+        <v>-28036.073493</v>
       </c>
       <c r="D45">
-        <v>1628.9064289999999</v>
+        <v>1628.2560000000001</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="B46">
-        <v>68509.286198999995</v>
+        <v>-77579.615351</v>
       </c>
       <c r="C46">
-        <v>-45995.970265999997</v>
+        <v>-28155.709814000002</v>
       </c>
       <c r="D46">
-        <v>1628.917469</v>
+        <v>1628.148584</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="B47">
-        <v>68247.034484999996</v>
+        <v>-77744.261958999996</v>
       </c>
       <c r="C47">
-        <v>-45838.241118999998</v>
+        <v>-27767.737729</v>
       </c>
       <c r="D47">
-        <v>1628.8522840000001</v>
+        <v>1628.1067069999999</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B48">
-        <v>68116.182514999993</v>
+        <v>-77462.560352999993</v>
       </c>
       <c r="C48">
-        <v>-46056.188383000001</v>
+        <v>-27648.253354</v>
       </c>
       <c r="D48">
-        <v>1628.826292</v>
+        <v>1628.232483</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="B49">
-        <v>68378.360486000005</v>
+        <v>-77923.095979999998</v>
       </c>
       <c r="C49">
-        <v>-46214.057059999999</v>
+        <v>-27116.739903999998</v>
       </c>
       <c r="D49">
-        <v>1628.9117189999999</v>
+        <v>1628.23198</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B50">
-        <v>68161.109280000004</v>
+        <v>-77947.002930000002</v>
       </c>
       <c r="C50">
-        <v>-46575.434178000003</v>
+        <v>-27056.223071</v>
       </c>
       <c r="D50">
-        <v>1628.9455359999999</v>
+        <v>1628.244655</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="B51">
-        <v>67898.977175000007</v>
+        <v>-78089.034698999996</v>
       </c>
       <c r="C51">
-        <v>-46417.513631000002</v>
+        <v>-26046.382328</v>
       </c>
       <c r="D51">
-        <v>1628.81466</v>
+        <v>1628.1973620000001</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="B52">
-        <v>67705.125690999994</v>
+        <v>-78376.177964000002</v>
       </c>
       <c r="C52">
-        <v>-47156.804723000001</v>
+        <v>-26152.224299000001</v>
       </c>
       <c r="D52">
-        <v>1629.0748309999999</v>
+        <v>1628.1663960000001</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="B53">
-        <v>67739.638967000006</v>
+        <v>-78954.509722000003</v>
       </c>
       <c r="C53">
-        <v>-47102.551033999996</v>
+        <v>-24583.878002000001</v>
       </c>
       <c r="D53">
-        <v>1629.0595249999999</v>
+        <v>1628.185737</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="B54">
-        <v>58806.371709999999</v>
+        <v>-78667.319778000005</v>
       </c>
       <c r="C54">
-        <v>57502.960662999998</v>
+        <v>-24478.145370999999</v>
       </c>
       <c r="D54">
-        <v>1629.2297100000001</v>
+        <v>1628.1688590000001</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="B55">
-        <v>59037.39157</v>
+        <v>-81460.423230999993</v>
       </c>
       <c r="C55">
-        <v>57703.610570999997</v>
+        <v>13110.330597</v>
       </c>
       <c r="D55">
-        <v>1629.460748</v>
+        <v>1628.9429889999999</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B56">
-        <v>59314.118141999999</v>
+        <v>-81447.441390000007</v>
       </c>
       <c r="C56">
-        <v>57385.651165000003</v>
+        <v>13172.929641000001</v>
       </c>
       <c r="D56">
-        <v>1629.518362</v>
+        <v>1628.9507819999999</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="B57">
-        <v>59083.248058999998</v>
+        <v>-81086.356163000004</v>
       </c>
       <c r="C57">
-        <v>57184.844348999999</v>
+        <v>13776.656292</v>
       </c>
       <c r="D57">
-        <v>1629.262097</v>
+        <v>1628.7394469999999</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B58">
-        <v>58487.463204</v>
+        <v>-81384.521024000001</v>
       </c>
       <c r="C58">
-        <v>58197.075733999998</v>
+        <v>13845.461262000001</v>
       </c>
       <c r="D58">
-        <v>1629.471955</v>
+        <v>1628.7231589999999</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="B59">
-        <v>58530.615491999997</v>
+        <v>-81289.696282999997</v>
       </c>
       <c r="C59">
-        <v>58149.437919999997</v>
+        <v>14256.557881999999</v>
       </c>
       <c r="D59">
-        <v>1629.4873319999999</v>
+        <v>1628.734031</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="B60">
-        <v>-72511.853860000003</v>
+        <v>-80991.551172000007</v>
       </c>
       <c r="C60">
-        <v>38739.911028000002</v>
+        <v>14187.539959</v>
       </c>
       <c r="D60">
-        <v>1628.6112499999999</v>
+        <v>1628.670351</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61">
-        <v>-72774.077514999997</v>
+        <v>-72511.853860000003</v>
       </c>
       <c r="C61">
-        <v>38897.635393999997</v>
+        <v>38739.911028000002</v>
       </c>
       <c r="D61">
-        <v>1628.5737799999999</v>
+        <v>1628.6112499999999</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
-        <v>-72525.667291000005</v>
+        <v>-72774.077514999997</v>
       </c>
       <c r="C62">
-        <v>39311.003338000002</v>
+        <v>38897.635393999997</v>
       </c>
       <c r="D62">
-        <v>1628.604576</v>
+        <v>1628.5737799999999</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
-        <v>-72263.444115999999</v>
+        <v>-72525.667291000005</v>
       </c>
       <c r="C63">
-        <v>39153.251086999997</v>
+        <v>39311.003338000002</v>
       </c>
       <c r="D63">
-        <v>1628.564376</v>
+        <v>1628.604576</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64">
-        <v>-63427.944858000003</v>
+        <v>-72263.444115999999</v>
       </c>
       <c r="C64">
-        <v>52635.539619000003</v>
+        <v>39153.251086999997</v>
       </c>
       <c r="D64">
-        <v>1751.4408679999999</v>
+        <v>1628.564376</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65">
-        <v>-63683.745897000001</v>
+        <v>-63427.944858000003</v>
       </c>
       <c r="C65">
-        <v>52850.395393999999</v>
+        <v>52635.539619000003</v>
       </c>
       <c r="D65">
-        <v>1751.425416</v>
+        <v>1751.4408679999999</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66">
-        <v>-63105.989667000002</v>
+        <v>-63683.745897000001</v>
       </c>
       <c r="C66">
-        <v>53539.042673999997</v>
+        <v>52850.395393999999</v>
       </c>
       <c r="D66">
-        <v>1751.4194769999999</v>
+        <v>1751.425416</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67">
-        <v>-62850.094974</v>
+        <v>-63105.989667000002</v>
       </c>
       <c r="C67">
-        <v>53324.205044000002</v>
+        <v>53539.042673999997</v>
       </c>
       <c r="D67">
-        <v>1751.4460260000001</v>
+        <v>1751.4194769999999</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68">
-        <v>58487.689560999999</v>
+        <v>-62850.094974</v>
       </c>
       <c r="C68">
-        <v>58197.189558999999</v>
+        <v>53324.205044000002</v>
       </c>
       <c r="D68">
-        <v>1629.536321</v>
+        <v>1751.4460260000001</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="B69">
-        <v>58530.817411000004</v>
+        <v>22033.491517999999</v>
       </c>
       <c r="C69">
-        <v>58149.565238000003</v>
+        <v>79180.812938000003</v>
       </c>
       <c r="D69">
-        <v>1629.535817</v>
+        <v>1629.1036240000001</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="B70">
-        <v>58806.460844000001</v>
+        <v>22102.589832999998</v>
       </c>
       <c r="C70">
-        <v>57503.025341</v>
+        <v>79478.919926000002</v>
       </c>
       <c r="D70">
-        <v>1629.426166</v>
+        <v>1629.1156040000001</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>151</v>
       </c>
       <c r="B71">
-        <v>59037.534226999996</v>
+        <v>22571.996546999999</v>
       </c>
       <c r="C71">
-        <v>57703.628626999998</v>
+        <v>79370.477775000007</v>
       </c>
       <c r="D71">
-        <v>1629.4045719999999</v>
+        <v>1629.1289770000001</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="B72">
-        <v>59314.191181000002</v>
+        <v>22503.148338999999</v>
       </c>
       <c r="C72">
-        <v>57385.597705</v>
+        <v>79072.331510000004</v>
       </c>
       <c r="D72">
-        <v>1629.4507020000001</v>
+        <v>1629.1209120000001</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="B73">
-        <v>59083.278117000002</v>
+        <v>22752.665624000001</v>
       </c>
       <c r="C73">
-        <v>57184.837161000003</v>
+        <v>79014.752340999999</v>
       </c>
       <c r="D73">
-        <v>1629.441026</v>
+        <v>1629.148279</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>146</v>
       </c>
       <c r="B74">
-        <v>-70419.250453000001</v>
+        <v>22821.524309</v>
       </c>
       <c r="C74">
-        <v>-43472.800956999999</v>
+        <v>79312.951335999998</v>
       </c>
       <c r="D74">
-        <v>1751.0736810000001</v>
+        <v>1629.183473</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="B75">
-        <v>-69942.920217000006</v>
+        <v>23232.82129</v>
       </c>
       <c r="C75">
-        <v>-44235.105387000003</v>
+        <v>79217.858489999999</v>
       </c>
       <c r="D75">
-        <v>1751.118068</v>
+        <v>1629.1887650000001</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="B76">
-        <v>-70136.025787999999</v>
+        <v>23163.854637</v>
       </c>
       <c r="C76">
-        <v>-43295.830716999997</v>
+        <v>78919.739006000003</v>
       </c>
       <c r="D76">
-        <v>1751.108835</v>
+        <v>1629.1646370000001</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>147</v>
       </c>
       <c r="B77">
-        <v>-69659.704652999993</v>
+        <v>23864.050051999999</v>
       </c>
       <c r="C77">
-        <v>-44058.14273</v>
+        <v>78980.032269000003</v>
       </c>
       <c r="D77">
-        <v>1751.102801</v>
+        <v>1629.385061</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="B78">
-        <v>-74595.592084999997</v>
+        <v>23927.188027</v>
       </c>
       <c r="C78">
-        <v>-35185.186755000002</v>
+        <v>78963.735344999994</v>
       </c>
       <c r="D78">
-        <v>1628.0697849999999</v>
+        <v>1629.420609</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="B79">
-        <v>-74313.862127</v>
+        <v>30458.500725999998</v>
       </c>
       <c r="C79">
-        <v>-35065.813776000003</v>
+        <v>76589.189723999996</v>
       </c>
       <c r="D79">
-        <v>1628.1010679999999</v>
+        <v>1752.2201419999999</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="B80">
-        <v>-74243.947371999995</v>
+        <v>30583.720659999999</v>
       </c>
       <c r="C80">
-        <v>-36013.728722</v>
+        <v>76898.888162000003</v>
       </c>
       <c r="D80">
-        <v>1628.1087769999999</v>
+        <v>1752.278787</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="B81">
-        <v>-73962.438330999998</v>
+        <v>31417.192405000002</v>
       </c>
       <c r="C81">
-        <v>-35893.836522999998</v>
+        <v>76562.176359999998</v>
       </c>
       <c r="D81">
-        <v>1628.112554</v>
+        <v>1752.2262900000001</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="B82">
-        <v>-77198.235436000003</v>
+        <v>31291.988700000002</v>
       </c>
       <c r="C82">
-        <v>-28270.681487999998</v>
+        <v>76252.474925000002</v>
       </c>
       <c r="D82">
-        <v>1628.182867</v>
+        <v>1752.222</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>200</v>
       </c>
       <c r="B83">
-        <v>-76846.744223000002</v>
+        <v>45066.201516000001</v>
       </c>
       <c r="C83">
-        <v>-29099.072069000002</v>
+        <v>68710.854882</v>
       </c>
       <c r="D83">
-        <v>1628.1673699999999</v>
+        <v>1629.427825</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>201</v>
       </c>
       <c r="B84">
-        <v>-77479.950614999994</v>
+        <v>45223.953046000002</v>
       </c>
       <c r="C84">
-        <v>-28390.141823000002</v>
+        <v>68973.056509999995</v>
       </c>
       <c r="D84">
-        <v>1628.107591</v>
+        <v>1629.4256069999999</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="B85">
-        <v>-77128.394448000006</v>
+        <v>45995.269998000003</v>
       </c>
       <c r="C85">
-        <v>-29218.636632000002</v>
+        <v>68509.571150000003</v>
       </c>
       <c r="D85">
-        <v>1628.0975370000001</v>
+        <v>1629.42221</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>203</v>
       </c>
       <c r="B86">
-        <v>-77923.095979999998</v>
+        <v>45837.512692999997</v>
       </c>
       <c r="C86">
-        <v>-27116.739903999998</v>
+        <v>68247.345621999993</v>
       </c>
       <c r="D86">
-        <v>1628.23198</v>
+        <v>1629.4140809999999</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="B87">
-        <v>-77947.002930000002</v>
+        <v>54032.953302000002</v>
       </c>
       <c r="C87">
-        <v>-27056.223071</v>
+        <v>62287.314006000001</v>
       </c>
       <c r="D87">
-        <v>1628.244655</v>
+        <v>1629.4765400000001</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="B88">
-        <v>-77462.560352999993</v>
+        <v>54238.329550000002</v>
       </c>
       <c r="C88">
-        <v>-27648.253354</v>
+        <v>62514.135587999997</v>
       </c>
       <c r="D88">
-        <v>1628.232483</v>
+        <v>1629.560052</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>136</v>
       </c>
       <c r="B89">
-        <v>-77297.975154</v>
+        <v>55233.866646000002</v>
       </c>
       <c r="C89">
-        <v>-28036.073493</v>
+        <v>61613.181835000003</v>
       </c>
       <c r="D89">
-        <v>1628.2560000000001</v>
+        <v>1629.5485430000001</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="B90">
-        <v>-77579.615351</v>
+        <v>55028.591060999999</v>
       </c>
       <c r="C90">
-        <v>-28155.709814000002</v>
+        <v>61386.247968999996</v>
       </c>
       <c r="D90">
-        <v>1628.148584</v>
+        <v>1629.4729279999999</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="B91">
-        <v>-77744.261958999996</v>
+        <v>55847.245521999997</v>
       </c>
       <c r="C91">
-        <v>-27767.737729</v>
+        <v>60935.54522</v>
       </c>
       <c r="D91">
-        <v>1628.1067069999999</v>
+        <v>1629.551164</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="B92">
-        <v>-78667.319778000005</v>
+        <v>56095.259278999998</v>
       </c>
       <c r="C92">
-        <v>-24478.145370999999</v>
+        <v>60694.367589000001</v>
       </c>
       <c r="D92">
-        <v>1628.1688590000001</v>
+        <v>1629.5133040000001</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="B93">
-        <v>-78089.034698999996</v>
+        <v>55570.548622000002</v>
       </c>
       <c r="C93">
-        <v>-26046.382328</v>
+        <v>61205.929828</v>
       </c>
       <c r="D93">
-        <v>1628.1973620000001</v>
+        <v>1629.5062439999999</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
       <c r="B94">
-        <v>-78376.177964000002</v>
+        <v>55759.502480000003</v>
       </c>
       <c r="C94">
-        <v>-26152.224299000001</v>
+        <v>60606.526401000003</v>
       </c>
       <c r="D94">
-        <v>1628.1663960000001</v>
+        <v>1629.441415</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="B95">
-        <v>-78954.509722000003</v>
+        <v>56363.183471999997</v>
       </c>
       <c r="C95">
-        <v>-24583.878002000001</v>
+        <v>60435.596838999998</v>
       </c>
       <c r="D95">
-        <v>1628.185737</v>
+        <v>1629.48504</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>183</v>
       </c>
       <c r="B96">
-        <v>-73862.787184000001</v>
+        <v>56485.295059999997</v>
       </c>
       <c r="C96">
-        <v>-36128.519823000002</v>
+        <v>59975.628676</v>
       </c>
       <c r="D96">
-        <v>1628.0574509999999</v>
+        <v>1629.46126</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>182</v>
       </c>
       <c r="B97">
-        <v>-73697.953878</v>
+        <v>56706.658450000003</v>
       </c>
       <c r="C97">
-        <v>-36516.922000999999</v>
+        <v>60186.983053000004</v>
       </c>
       <c r="D97">
-        <v>1628.1123170000001</v>
+        <v>1629.4439669999999</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>185</v>
       </c>
       <c r="B98">
-        <v>-73979.705845999997</v>
+        <v>57862.991992000003</v>
       </c>
       <c r="C98">
-        <v>-36636.337194</v>
+        <v>58979.417130000002</v>
       </c>
       <c r="D98">
-        <v>1628.0378969999999</v>
+        <v>1629.520395</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>184</v>
       </c>
       <c r="B99">
-        <v>-74144.553941999999</v>
+        <v>57641.846234999997</v>
       </c>
       <c r="C99">
-        <v>-36247.983831999998</v>
+        <v>58767.945330000002</v>
       </c>
       <c r="D99">
-        <v>1628.072355</v>
+        <v>1629.4915309999999</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="B100">
-        <v>-73608.967923000004</v>
+        <v>58487.689560999999</v>
       </c>
       <c r="C100">
-        <v>-37276.056831000002</v>
+        <v>58197.189558999999</v>
       </c>
       <c r="D100">
-        <v>1628.306456</v>
+        <v>1629.536321</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="B101">
-        <v>-73635.643284000005</v>
+        <v>58530.817411000004</v>
       </c>
       <c r="C101">
-        <v>-37217.039360000002</v>
+        <v>58149.565238000003</v>
       </c>
       <c r="D101">
-        <v>1628.2867759999999</v>
+        <v>1629.535817</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="B102">
-        <v>-50311.882017999997</v>
+        <v>58806.460844000001</v>
       </c>
       <c r="C102">
-        <v>-65579.884220000007</v>
+        <v>57503.025341</v>
       </c>
       <c r="D102">
-        <v>1628.466093</v>
+        <v>1629.426166</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="B103">
-        <v>-50031.325087999998</v>
+        <v>59037.534226999996</v>
       </c>
       <c r="C103">
-        <v>-65782.288986</v>
+        <v>57703.628626999998</v>
       </c>
       <c r="D103">
-        <v>1628.5078619999999</v>
+        <v>1629.4045719999999</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="B104">
-        <v>-49995.558626999999</v>
+        <v>59314.191181000002</v>
       </c>
       <c r="C104">
-        <v>-65441.839439000003</v>
+        <v>57385.597705</v>
       </c>
       <c r="D104">
-        <v>1628.3685640000001</v>
+        <v>1629.4507020000001</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="B105">
-        <v>-49683.837793999999</v>
+        <v>59083.278117000002</v>
       </c>
       <c r="C105">
-        <v>-66033.140010999996</v>
+        <v>57184.837161000003</v>
       </c>
       <c r="D105">
-        <v>1628.4670470000001</v>
+        <v>1629.441026</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>105</v>
+        <v>189</v>
       </c>
       <c r="B106">
-        <v>-50658.465701000001</v>
+        <v>59250.333879999998</v>
       </c>
       <c r="C106">
-        <v>-65329.963500999998</v>
+        <v>56992.42355</v>
       </c>
       <c r="D106">
-        <v>1628.416545</v>
+        <v>1629.489137</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>186</v>
       </c>
       <c r="B107">
-        <v>-52145.941112</v>
+        <v>59481.377761000003</v>
       </c>
       <c r="C107">
-        <v>-64269.652409000002</v>
+        <v>57193.106644</v>
       </c>
       <c r="D107">
-        <v>1628.482393</v>
+        <v>1629.5349160000001</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>187</v>
       </c>
       <c r="B108">
-        <v>-51085.779866999997</v>
+        <v>60071.733393000002</v>
       </c>
       <c r="C108">
-        <v>-65093.474029999998</v>
+        <v>56514.07905</v>
       </c>
       <c r="D108">
-        <v>1628.416444</v>
+        <v>1629.4889539999999</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>188</v>
       </c>
       <c r="B109">
-        <v>-50897.876967999997</v>
+        <v>59840.539638000002</v>
       </c>
       <c r="C109">
-        <v>-64851.905810999997</v>
+        <v>56313.521492</v>
       </c>
       <c r="D109">
-        <v>1628.379619</v>
+        <v>1629.448703</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="B110">
-        <v>-51958.052589999999</v>
+        <v>64850.487965</v>
       </c>
       <c r="C110">
-        <v>-64028.130054000001</v>
+        <v>50550.041297000003</v>
       </c>
       <c r="D110">
-        <v>1628.3734019999999</v>
+        <v>1629.27935</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>193</v>
       </c>
       <c r="B111">
-        <v>-81460.423230999993</v>
+        <v>65081.683587</v>
       </c>
       <c r="C111">
-        <v>13110.330597</v>
+        <v>50750.554925999997</v>
       </c>
       <c r="D111">
-        <v>1628.9429889999999</v>
+        <v>1629.292776</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
       <c r="B112">
-        <v>-81447.441390000007</v>
+        <v>65358.187462000002</v>
       </c>
       <c r="C112">
-        <v>13172.929641000001</v>
+        <v>50432.48846</v>
       </c>
       <c r="D112">
-        <v>1628.9507819999999</v>
+        <v>1629.345415</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>112</v>
+        <v>191</v>
       </c>
       <c r="B113">
-        <v>-81086.356163000004</v>
+        <v>65127.136159000001</v>
       </c>
       <c r="C113">
-        <v>13776.656292</v>
+        <v>50231.838755999997</v>
       </c>
       <c r="D113">
-        <v>1628.7394469999999</v>
+        <v>1629.2896969999999</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>195</v>
       </c>
       <c r="B114">
-        <v>-80991.551172000007</v>
+        <v>65729.343378999998</v>
       </c>
       <c r="C114">
-        <v>14187.539959</v>
+        <v>49868.979699000003</v>
       </c>
       <c r="D114">
-        <v>1628.670351</v>
+        <v>1629.55582</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>194</v>
       </c>
       <c r="B115">
-        <v>-81289.696282999997</v>
+        <v>65770.989446000007</v>
       </c>
       <c r="C115">
-        <v>14256.557881999999</v>
+        <v>49818.598553999997</v>
       </c>
       <c r="D115">
-        <v>1628.734031</v>
+        <v>1629.5417010000001</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>115</v>
+        <v>199</v>
       </c>
       <c r="B116">
-        <v>-81384.521024000001</v>
+        <v>66218.352562999993</v>
       </c>
       <c r="C116">
-        <v>13845.461262000001</v>
+        <v>48901.380145000003</v>
       </c>
       <c r="D116">
-        <v>1628.7231589999999</v>
+        <v>1629.380257</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>198</v>
       </c>
       <c r="B117">
-        <v>80188.771439999997</v>
+        <v>66459.058248999994</v>
       </c>
       <c r="C117">
-        <v>20455.803443000001</v>
+        <v>49090.378942000003</v>
       </c>
       <c r="D117">
-        <v>1751.7081430000001</v>
+        <v>1629.371404</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>197</v>
       </c>
       <c r="B118">
-        <v>80406.291612000001</v>
+        <v>67493.248152</v>
       </c>
       <c r="C118">
-        <v>19583.613438</v>
+        <v>47778.155313000003</v>
       </c>
       <c r="D118">
-        <v>1751.5881099999999</v>
+        <v>1629.3095599999999</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>196</v>
       </c>
       <c r="B119">
-        <v>80082.171004999997</v>
+        <v>67252.772683000003</v>
       </c>
       <c r="C119">
-        <v>19502.791150000001</v>
+        <v>47588.86894</v>
       </c>
       <c r="D119">
-        <v>1751.6266419999999</v>
+        <v>1629.2763110000001</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
       <c r="B120">
-        <v>79864.653921000005</v>
+        <v>73608.770881999997</v>
       </c>
       <c r="C120">
-        <v>20374.942508</v>
+        <v>37274.857794000003</v>
       </c>
       <c r="D120">
-        <v>1751.6513219999999</v>
+        <v>1629.200585</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="B121">
-        <v>81086.467745999995</v>
+        <v>73635.324869000004</v>
       </c>
       <c r="C121">
-        <v>-13776.845754</v>
+        <v>37216.005539999998</v>
       </c>
       <c r="D121">
-        <v>1628.5691179999999</v>
+        <v>1629.1920150000001</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="B122">
-        <v>80991.631586000003</v>
+        <v>73697.872711000004</v>
       </c>
       <c r="C122">
-        <v>-14187.699194999999</v>
+        <v>36515.557012999998</v>
       </c>
       <c r="D122">
-        <v>1628.626062</v>
+        <v>1629.039628</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>213</v>
       </c>
       <c r="B123">
-        <v>81289.750050000002</v>
+        <v>73979.585307000001</v>
       </c>
       <c r="C123">
-        <v>-14256.651997999999</v>
+        <v>36635.028830000003</v>
       </c>
       <c r="D123">
-        <v>1628.5972810000001</v>
+        <v>1629.0476160000001</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>212</v>
       </c>
       <c r="B124">
-        <v>81384.595161999998</v>
+        <v>74144.397203999994</v>
       </c>
       <c r="C124">
-        <v>-13845.758661</v>
+        <v>36246.825122000002</v>
       </c>
       <c r="D124">
-        <v>1628.5614740000001</v>
+        <v>1629.0436850000001</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>211</v>
       </c>
       <c r="B125">
-        <v>81460.577646000005</v>
+        <v>73862.664378999994</v>
       </c>
       <c r="C125">
-        <v>-13110.684767000001</v>
+        <v>36127.337134000001</v>
       </c>
       <c r="D125">
-        <v>1628.6619439999999</v>
+        <v>1629.0466329999999</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B126">
-        <v>81447.459323999996</v>
+        <v>79864.653921000005</v>
       </c>
       <c r="C126">
-        <v>-13174.032131</v>
+        <v>20374.942508</v>
       </c>
       <c r="D126">
-        <v>1628.6825080000001</v>
+        <v>1751.6513219999999</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="B127">
-        <v>78919.213329000006</v>
+        <v>80188.771439999997</v>
       </c>
       <c r="C127">
-        <v>-23164.422753999999</v>
+        <v>20455.803443000001</v>
       </c>
       <c r="D127">
-        <v>1628.7486220000001</v>
+        <v>1751.7081430000001</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B128">
-        <v>79014.058717000007</v>
+        <v>80406.291612000001</v>
       </c>
       <c r="C128">
-        <v>-22753.458895</v>
+        <v>19583.613438</v>
       </c>
       <c r="D128">
-        <v>1628.764776</v>
+        <v>1751.5881099999999</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B129">
-        <v>79312.218938000005</v>
+        <v>80082.171004999997</v>
       </c>
       <c r="C129">
-        <v>-22822.436987000001</v>
+        <v>19502.791150000001</v>
       </c>
       <c r="D129">
-        <v>1628.8209409999999</v>
+        <v>1751.6266419999999</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>129</v>
+        <v>180</v>
       </c>
       <c r="B130">
-        <v>79217.348203000001</v>
+        <v>82626.827546999994</v>
       </c>
       <c r="C130">
-        <v>-23233.305733000001</v>
+        <v>-1810.527603</v>
       </c>
       <c r="D130">
-        <v>1628.7573050000001</v>
+        <v>1628.6008750000001</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>181</v>
       </c>
       <c r="B131">
-        <v>78963.606102000005</v>
+        <v>82627.947952000002</v>
       </c>
       <c r="C131">
-        <v>-23927.731875000001</v>
+        <v>-2156.1425239999999</v>
       </c>
       <c r="D131">
-        <v>1628.910177</v>
+        <v>1628.6580300000001</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>131</v>
+        <v>179</v>
       </c>
       <c r="B132">
-        <v>78979.725663999998</v>
+        <v>82630.808011000001</v>
       </c>
       <c r="C132">
-        <v>-23864.789041</v>
+        <v>-1581.957903</v>
       </c>
       <c r="D132">
-        <v>1628.9008779999999</v>
+        <v>1628.5489110000001</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>132</v>
+        <v>178</v>
       </c>
       <c r="B133">
-        <v>-53323.315569999999</v>
+        <v>82330.204289000001</v>
       </c>
       <c r="C133">
-        <v>-62850.201738000003</v>
+        <v>-1975.588853</v>
       </c>
       <c r="D133">
-        <v>1751.3973960000001</v>
+        <v>1628.485897</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>133</v>
+        <v>177</v>
       </c>
       <c r="B134">
-        <v>-52634.707397999999</v>
+        <v>82630.884179000001</v>
       </c>
       <c r="C134">
-        <v>-63427.906902000002</v>
+        <v>-2509.516102</v>
       </c>
       <c r="D134">
-        <v>1751.4253920000001</v>
+        <v>1628.6043669999999</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>134</v>
+        <v>30</v>
       </c>
       <c r="B135">
-        <v>-52849.422150999999</v>
+        <v>81722.469494999998</v>
       </c>
       <c r="C135">
-        <v>-63683.749931999999</v>
+        <v>-10445.656853</v>
       </c>
       <c r="D135">
-        <v>1751.404198</v>
+        <v>1628.573234</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>135</v>
+        <v>31</v>
       </c>
       <c r="B136">
-        <v>-53538.076654999997</v>
+        <v>82023.565625999996</v>
       </c>
       <c r="C136">
-        <v>-63106.050764</v>
+        <v>-10500.228024</v>
       </c>
       <c r="D136">
-        <v>1751.355157</v>
+        <v>1628.601887</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="B137">
-        <v>30458.500725999998</v>
+        <v>81726.368868999998</v>
       </c>
       <c r="C137">
-        <v>76589.189723999996</v>
+        <v>-12145.191948</v>
       </c>
       <c r="D137">
-        <v>1752.2201419999999</v>
+        <v>1628.5951439999999</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>137</v>
+        <v>33</v>
       </c>
       <c r="B138">
-        <v>31291.988700000002</v>
+        <v>81425.250121999998</v>
       </c>
       <c r="C138">
-        <v>76252.474925000002</v>
+        <v>-12090.67841</v>
       </c>
       <c r="D138">
-        <v>1752.222</v>
+        <v>1628.595687</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="B139">
-        <v>31417.192405000002</v>
+        <v>81460.577646000005</v>
       </c>
       <c r="C139">
-        <v>76562.176359999998</v>
+        <v>-13110.684767000001</v>
       </c>
       <c r="D139">
-        <v>1752.2262900000001</v>
+        <v>1628.6619439999999</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="B140">
-        <v>30583.720659999999</v>
+        <v>81447.459323999996</v>
       </c>
       <c r="C140">
-        <v>76898.888162000003</v>
+        <v>-13174.032131</v>
       </c>
       <c r="D140">
-        <v>1752.278787</v>
+        <v>1628.6825080000001</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="B141">
-        <v>55028.591060999999</v>
+        <v>81086.467745999995</v>
       </c>
       <c r="C141">
-        <v>61386.247968999996</v>
+        <v>-13776.845754</v>
       </c>
       <c r="D141">
-        <v>1629.4729279999999</v>
+        <v>1628.5691179999999</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B142">
-        <v>54032.953302000002</v>
+        <v>81384.595161999998</v>
       </c>
       <c r="C142">
-        <v>62287.314006000001</v>
+        <v>-13845.758661</v>
       </c>
       <c r="D142">
-        <v>1629.4765400000001</v>
+        <v>1628.5614740000001</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="B143">
-        <v>55233.866646000002</v>
+        <v>81289.750050000002</v>
       </c>
       <c r="C143">
-        <v>61613.181835000003</v>
+        <v>-14256.651997999999</v>
       </c>
       <c r="D143">
-        <v>1629.5485430000001</v>
+        <v>1628.5972810000001</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="B144">
-        <v>54238.329550000002</v>
+        <v>80991.631586000003</v>
       </c>
       <c r="C144">
-        <v>62514.135587999997</v>
+        <v>-14187.699194999999</v>
       </c>
       <c r="D144">
-        <v>1629.560052</v>
+        <v>1628.626062</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="B145">
-        <v>56095.259278999998</v>
+        <v>80934.330642000001</v>
       </c>
       <c r="C145">
-        <v>60694.367589000001</v>
+        <v>-14436.102134999999</v>
       </c>
       <c r="D145">
-        <v>1629.5133040000001</v>
+        <v>1628.5660640000001</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>145</v>
+        <v>1</v>
       </c>
       <c r="B146">
-        <v>55847.245521999997</v>
+        <v>81232.481304000001</v>
       </c>
       <c r="C146">
-        <v>60935.54522</v>
+        <v>-14504.922973999999</v>
       </c>
       <c r="D146">
-        <v>1629.551164</v>
+        <v>1628.6097130000001</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>146</v>
+        <v>2</v>
       </c>
       <c r="B147">
-        <v>55570.548622000002</v>
+        <v>81030.198696000007</v>
       </c>
       <c r="C147">
-        <v>61205.929828</v>
+        <v>-15381.054975999999</v>
       </c>
       <c r="D147">
-        <v>1629.5062439999999</v>
+        <v>1628.6197770000001</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>3</v>
       </c>
       <c r="B148">
-        <v>56363.183471999997</v>
+        <v>80732.026761999994</v>
       </c>
       <c r="C148">
-        <v>60435.596838999998</v>
+        <v>-15312.466528999999</v>
       </c>
       <c r="D148">
-        <v>1629.48504</v>
+        <v>1628.6192980000001</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>148</v>
+        <v>4</v>
       </c>
       <c r="B149">
-        <v>55759.502480000003</v>
+        <v>79274.066523000001</v>
       </c>
       <c r="C149">
-        <v>60606.526401000003</v>
+        <v>-21628.189342000001</v>
       </c>
       <c r="D149">
-        <v>1629.441415</v>
+        <v>1628.6438430000001</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>149</v>
+        <v>5</v>
       </c>
       <c r="B150">
-        <v>22752.665624000001</v>
+        <v>79572.198252000002</v>
       </c>
       <c r="C150">
-        <v>79014.752340999999</v>
+        <v>-21697.032078</v>
       </c>
       <c r="D150">
-        <v>1629.148279</v>
+        <v>1628.6916859999999</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>150</v>
+        <v>6</v>
       </c>
       <c r="B151">
-        <v>23163.854637</v>
+        <v>79369.494451000006</v>
       </c>
       <c r="C151">
-        <v>78919.739006000003</v>
+        <v>-22574.335514999999</v>
       </c>
       <c r="D151">
-        <v>1629.1646370000001</v>
+        <v>1628.678774</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>151</v>
+        <v>7</v>
       </c>
       <c r="B152">
-        <v>23232.82129</v>
+        <v>79071.456109999999</v>
       </c>
       <c r="C152">
-        <v>79217.858489999999</v>
+        <v>-22505.008741000001</v>
       </c>
       <c r="D152">
-        <v>1629.1887650000001</v>
+        <v>1628.6178849999999</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="B153">
-        <v>22821.524309</v>
+        <v>79014.058717000007</v>
       </c>
       <c r="C153">
-        <v>79312.951335999998</v>
+        <v>-22753.458895</v>
       </c>
       <c r="D153">
-        <v>1629.183473</v>
+        <v>1628.764776</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="B154">
-        <v>23864.050051999999</v>
+        <v>79312.218938000005</v>
       </c>
       <c r="C154">
-        <v>78980.032269000003</v>
+        <v>-22822.436987000001</v>
       </c>
       <c r="D154">
-        <v>1629.385061</v>
+        <v>1628.8209409999999</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
       <c r="B155">
-        <v>23927.188027</v>
+        <v>79217.348203000001</v>
       </c>
       <c r="C155">
-        <v>78963.735344999994</v>
+        <v>-23233.305733000001</v>
       </c>
       <c r="D155">
-        <v>1629.420609</v>
+        <v>1628.7573050000001</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="B156">
-        <v>22033.491517999999</v>
+        <v>78919.213329000006</v>
       </c>
       <c r="C156">
-        <v>79180.812938000003</v>
+        <v>-23164.422753999999</v>
       </c>
       <c r="D156">
-        <v>1629.1036240000001</v>
+        <v>1628.7486220000001</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="B157">
-        <v>22503.148338999999</v>
+        <v>78979.725663999998</v>
       </c>
       <c r="C157">
-        <v>79072.331510000004</v>
+        <v>-23864.789041</v>
       </c>
       <c r="D157">
-        <v>1629.1209120000001</v>
+        <v>1628.9008779999999</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="B158">
-        <v>22571.996546999999</v>
+        <v>78963.606102000005</v>
       </c>
       <c r="C158">
-        <v>79370.477775000007</v>
+        <v>-23927.731875000001</v>
       </c>
       <c r="D158">
-        <v>1629.1289770000001</v>
+        <v>1628.910177</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>158</v>
+        <v>43</v>
       </c>
       <c r="B159">
-        <v>22102.589832999998</v>
+        <v>68710.525204999998</v>
       </c>
       <c r="C159">
-        <v>79478.919926000002</v>
+        <v>-45066.885010999998</v>
       </c>
       <c r="D159">
-        <v>1629.1156040000001</v>
+        <v>1628.8684479999999</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>159</v>
+        <v>44</v>
       </c>
       <c r="B160">
-        <v>61613.181449999996</v>
+        <v>68972.805871999997</v>
       </c>
       <c r="C160">
-        <v>-55234.285846999999</v>
+        <v>-45224.516497999997</v>
       </c>
       <c r="D160">
-        <v>1628.75352</v>
+        <v>1628.9064289999999</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>160</v>
+        <v>45</v>
       </c>
       <c r="B161">
-        <v>61386.478532000001</v>
+        <v>68509.286198999995</v>
       </c>
       <c r="C161">
-        <v>-55028.728410000003</v>
+        <v>-45995.970265999997</v>
       </c>
       <c r="D161">
-        <v>1628.718758</v>
+        <v>1628.917469</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>161</v>
+        <v>46</v>
       </c>
       <c r="B162">
-        <v>62287.444340000002</v>
+        <v>68247.034484999996</v>
       </c>
       <c r="C162">
-        <v>-54033.264458999998</v>
+        <v>-45838.241118999998</v>
       </c>
       <c r="D162">
-        <v>1628.79476</v>
+        <v>1628.8522840000001</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>162</v>
+        <v>47</v>
       </c>
       <c r="B163">
-        <v>62514.269633999997</v>
+        <v>68116.182514999993</v>
       </c>
       <c r="C163">
-        <v>-54238.671578000001</v>
+        <v>-46056.188383000001</v>
       </c>
       <c r="D163">
-        <v>1628.7846950000001</v>
+        <v>1628.826292</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>163</v>
+        <v>48</v>
       </c>
       <c r="B164">
-        <v>37276.184647000002</v>
+        <v>68378.360486000005</v>
       </c>
       <c r="C164">
-        <v>-73609.074445999999</v>
+        <v>-46214.057059999999</v>
       </c>
       <c r="D164">
-        <v>1628.139574</v>
+        <v>1628.9117189999999</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>164</v>
+        <v>49</v>
       </c>
       <c r="B165">
-        <v>37217.113251000002</v>
+        <v>68161.109280000004</v>
       </c>
       <c r="C165">
-        <v>-73635.723209999996</v>
+        <v>-46575.434178000003</v>
       </c>
       <c r="D165">
-        <v>1628.134816</v>
+        <v>1628.9455359999999</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>165</v>
+        <v>50</v>
       </c>
       <c r="B166">
-        <v>36128.535488000001</v>
+        <v>67898.977175000007</v>
       </c>
       <c r="C166">
-        <v>-73862.685796000005</v>
+        <v>-46417.513631000002</v>
       </c>
       <c r="D166">
-        <v>1628.0704330000001</v>
+        <v>1628.81466</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>166</v>
+        <v>52</v>
       </c>
       <c r="B167">
-        <v>36247.700392999999</v>
+        <v>67739.638967000006</v>
       </c>
       <c r="C167">
-        <v>-74144.615888</v>
+        <v>-47102.551033999996</v>
       </c>
       <c r="D167">
-        <v>1628.0841680000001</v>
+        <v>1629.0595249999999</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>167</v>
+        <v>51</v>
       </c>
       <c r="B168">
-        <v>36636.268090999998</v>
+        <v>67705.125690999994</v>
       </c>
       <c r="C168">
-        <v>-73979.697182000004</v>
+        <v>-47156.804723000001</v>
       </c>
       <c r="D168">
-        <v>1628.0651339999999</v>
+        <v>1629.0748309999999</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>168</v>
+        <v>8</v>
       </c>
       <c r="B169">
-        <v>36516.985098999998</v>
+        <v>66971.154806999999</v>
       </c>
       <c r="C169">
-        <v>-73697.874465999994</v>
+        <v>-47866.098901999998</v>
       </c>
       <c r="D169">
-        <v>1628.0910550000001</v>
+        <v>1628.799704</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>169</v>
+        <v>9</v>
       </c>
       <c r="B170">
-        <v>38212.722506999999</v>
+        <v>67225.510158999998</v>
       </c>
       <c r="C170">
-        <v>-73256.766138999999</v>
+        <v>-48036.269286000002</v>
       </c>
       <c r="D170">
-        <v>1628.0296820000001</v>
+        <v>1628.8840970000001</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="B171">
-        <v>39718.446564999998</v>
+        <v>66296.619153000007</v>
       </c>
       <c r="C171">
-        <v>-72530.282166000005</v>
+        <v>-49426.104474</v>
       </c>
       <c r="D171">
-        <v>1628.0704949999999</v>
+        <v>1628.886718</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>171</v>
+        <v>11</v>
       </c>
       <c r="B172">
-        <v>39585.376396</v>
+        <v>66042.137417000005</v>
       </c>
       <c r="C172">
-        <v>-72254.683655999994</v>
+        <v>-49256.099554</v>
       </c>
       <c r="D172">
-        <v>1628.1049169999999</v>
+        <v>1628.81059</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B173">
-        <v>38079.786076999997</v>
+        <v>65782.781541999997</v>
       </c>
       <c r="C173">
-        <v>-72981.155689000007</v>
+        <v>-50031.702222</v>
       </c>
       <c r="D173">
-        <v>1628.009865</v>
+        <v>1628.943207</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B174">
-        <v>66001.57991</v>
+        <v>65580.412068000005</v>
       </c>
       <c r="C174">
-        <v>-49730.692937</v>
+        <v>-50312.172086999999</v>
       </c>
       <c r="D174">
-        <v>1628.9033669999999</v>
+        <v>1628.9570920000001</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B175">
-        <v>65446.359065999997</v>
+        <v>66001.57991</v>
       </c>
       <c r="C175">
-        <v>-49990.188015</v>
+        <v>-49730.692937</v>
       </c>
       <c r="D175">
-        <v>1628.7547440000001</v>
+        <v>1628.9033669999999</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B176">
-        <v>65782.781541999997</v>
+        <v>65446.359065999997</v>
       </c>
       <c r="C176">
-        <v>-50031.702222</v>
+        <v>-49990.188015</v>
       </c>
       <c r="D176">
-        <v>1628.943207</v>
+        <v>1628.7547440000001</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B177">
-        <v>65580.412068000005</v>
+        <v>65436.065030999998</v>
       </c>
       <c r="C177">
-        <v>-50312.172086999999</v>
+        <v>-50519.043574000003</v>
       </c>
       <c r="D177">
-        <v>1628.9570920000001</v>
+        <v>1628.88813</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="B178">
-        <v>65436.065030999998</v>
+        <v>62287.444340000002</v>
       </c>
       <c r="C178">
-        <v>-50519.043574000003</v>
+        <v>-54033.264458999998</v>
       </c>
       <c r="D178">
-        <v>1628.88813</v>
+        <v>1628.79476</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="B179">
-        <v>46823.346484000002</v>
+        <v>62514.269633999997</v>
       </c>
       <c r="C179">
-        <v>-68115.125243000002</v>
+        <v>-54238.671578000001</v>
       </c>
       <c r="D179">
-        <v>1628.3950689999999</v>
+        <v>1628.7846950000001</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="B180">
-        <v>47102.404473000002</v>
+        <v>61613.181449999996</v>
       </c>
       <c r="C180">
-        <v>-67911.047248000003</v>
+        <v>-55234.285846999999</v>
       </c>
       <c r="D180">
-        <v>1628.4475199999999</v>
+        <v>1628.75352</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="B181">
-        <v>46800.595104</v>
+        <v>61386.478532000001</v>
       </c>
       <c r="C181">
-        <v>-67763.701304000002</v>
+        <v>-55028.728410000003</v>
       </c>
       <c r="D181">
-        <v>1628.3185149999999</v>
+        <v>1628.718758</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>181</v>
+        <v>12</v>
       </c>
       <c r="B182">
-        <v>46512.776766000003</v>
+        <v>59975.624873000001</v>
       </c>
       <c r="C182">
-        <v>-68343.406281999996</v>
+        <v>-56485.835679000003</v>
       </c>
       <c r="D182">
-        <v>1628.298303</v>
+        <v>1628.6832649999999</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>182</v>
+        <v>13</v>
       </c>
       <c r="B183">
-        <v>47389.648287000004</v>
+        <v>60187.260206999999</v>
       </c>
       <c r="C183">
-        <v>-67703.244080999997</v>
+        <v>-56706.876279999997</v>
       </c>
       <c r="D183">
-        <v>1628.445438</v>
+        <v>1628.7549819999999</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="B184">
-        <v>82630.884179000001</v>
+        <v>58980.168005</v>
       </c>
       <c r="C184">
-        <v>-2509.516102</v>
+        <v>-57862.651485000002</v>
       </c>
       <c r="D184">
-        <v>1628.6043669999999</v>
+        <v>1628.6924879999999</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>184</v>
+        <v>15</v>
       </c>
       <c r="B185">
-        <v>82330.204289000001</v>
+        <v>58768.585911000002</v>
       </c>
       <c r="C185">
-        <v>-1975.588853</v>
+        <v>-57641.555157000003</v>
       </c>
       <c r="D185">
-        <v>1628.485897</v>
+        <v>1628.6476580000001</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>185</v>
+        <v>20</v>
       </c>
       <c r="B186">
-        <v>82630.808011000001</v>
+        <v>58197.202144000003</v>
       </c>
       <c r="C186">
-        <v>-1581.957903</v>
+        <v>-58487.781667000003</v>
       </c>
       <c r="D186">
-        <v>1628.5489110000001</v>
+        <v>1628.795656</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>186</v>
+        <v>21</v>
       </c>
       <c r="B187">
-        <v>82626.827546999994</v>
+        <v>58149.543564</v>
       </c>
       <c r="C187">
-        <v>-1810.527603</v>
+        <v>-58531.026583999999</v>
       </c>
       <c r="D187">
-        <v>1628.6008750000001</v>
+        <v>1628.831459</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>187</v>
+        <v>17</v>
       </c>
       <c r="B188">
-        <v>82627.947952000002</v>
+        <v>57502.911726999999</v>
       </c>
       <c r="C188">
-        <v>-2156.1425239999999</v>
+        <v>-58807.101329999998</v>
       </c>
       <c r="D188">
-        <v>1628.6580300000001</v>
+        <v>1628.5749940000001</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>188</v>
+        <v>16</v>
       </c>
       <c r="B189">
-        <v>56706.658450000003</v>
+        <v>57703.702570000001</v>
       </c>
       <c r="C189">
-        <v>60186.983053000004</v>
+        <v>-59037.973052000001</v>
       </c>
       <c r="D189">
-        <v>1629.4439669999999</v>
+        <v>1628.7402850000001</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>189</v>
+        <v>19</v>
       </c>
       <c r="B190">
-        <v>56485.295059999997</v>
+        <v>57385.526585</v>
       </c>
       <c r="C190">
-        <v>59975.628676</v>
+        <v>-59314.733445999998</v>
       </c>
       <c r="D190">
-        <v>1629.46126</v>
+        <v>1628.7335860000001</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>190</v>
+        <v>18</v>
       </c>
       <c r="B191">
-        <v>57641.846234999997</v>
+        <v>57184.696201999999</v>
       </c>
       <c r="C191">
-        <v>58767.945330000002</v>
+        <v>-59083.803965999999</v>
       </c>
       <c r="D191">
-        <v>1629.4915309999999</v>
+        <v>1628.586728</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>191</v>
+        <v>23</v>
       </c>
       <c r="B192">
-        <v>57862.991992000003</v>
+        <v>48901.755111999999</v>
       </c>
       <c r="C192">
-        <v>58979.417130000002</v>
+        <v>-66218.760722999999</v>
       </c>
       <c r="D192">
-        <v>1629.520395</v>
+        <v>1628.3589380000001</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>192</v>
+        <v>24</v>
       </c>
       <c r="B193">
-        <v>59481.377761000003</v>
+        <v>49091.544134999996</v>
       </c>
       <c r="C193">
-        <v>57193.106644</v>
+        <v>-66458.810536999998</v>
       </c>
       <c r="D193">
-        <v>1629.5349160000001</v>
+        <v>1628.4045590000001</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>193</v>
+        <v>25</v>
       </c>
       <c r="B194">
-        <v>60071.733393000002</v>
+        <v>47778.567331999999</v>
       </c>
       <c r="C194">
-        <v>56514.07905</v>
+        <v>-67493.689155999993</v>
       </c>
       <c r="D194">
-        <v>1629.4889539999999</v>
+        <v>1628.384898</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>194</v>
+        <v>22</v>
       </c>
       <c r="B195">
-        <v>59840.539638000002</v>
+        <v>47589.051968</v>
       </c>
       <c r="C195">
-        <v>56313.521492</v>
+        <v>-67253.396653000003</v>
       </c>
       <c r="D195">
-        <v>1629.448703</v>
+        <v>1628.3378600000001</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="B196">
-        <v>59250.333879999998</v>
+        <v>47102.404473000002</v>
       </c>
       <c r="C196">
-        <v>56992.42355</v>
+        <v>-67911.047248000003</v>
       </c>
       <c r="D196">
-        <v>1629.489137</v>
+        <v>1628.4475199999999</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="B197">
-        <v>64850.487965</v>
+        <v>46823.346484000002</v>
       </c>
       <c r="C197">
-        <v>50550.041297000003</v>
+        <v>-68115.125243000002</v>
       </c>
       <c r="D197">
-        <v>1629.27935</v>
+        <v>1628.3950689999999</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="B198">
-        <v>65127.136159000001</v>
+        <v>47389.648287000004</v>
       </c>
       <c r="C198">
-        <v>50231.838755999997</v>
+        <v>-67703.244080999997</v>
       </c>
       <c r="D198">
-        <v>1629.2896969999999</v>
+        <v>1628.445438</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="B199">
-        <v>65358.187462000002</v>
+        <v>46800.595104</v>
       </c>
       <c r="C199">
-        <v>50432.48846</v>
+        <v>-67763.701304000002</v>
       </c>
       <c r="D199">
-        <v>1629.345415</v>
+        <v>1628.3185149999999</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="B200">
-        <v>65081.683587</v>
+        <v>46512.776766000003</v>
       </c>
       <c r="C200">
-        <v>50750.554925999997</v>
+        <v>-68343.406281999996</v>
       </c>
       <c r="D200">
-        <v>1629.292776</v>
+        <v>1628.298303</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>200</v>
+        <v>26</v>
       </c>
       <c r="B201">
-        <v>65770.989446000007</v>
+        <v>44057.660012</v>
       </c>
       <c r="C201">
-        <v>49818.598553999997</v>
+        <v>-69660.147303000005</v>
       </c>
       <c r="D201">
-        <v>1629.5417010000001</v>
+        <v>1751.219542</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>201</v>
+        <v>27</v>
       </c>
       <c r="B202">
-        <v>65729.343378999998</v>
+        <v>44234.664687999997</v>
       </c>
       <c r="C202">
-        <v>49868.979699000003</v>
+        <v>-69943.440128000002</v>
       </c>
       <c r="D202">
-        <v>1629.55582</v>
+        <v>1751.2733020000001</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>202</v>
+        <v>28</v>
       </c>
       <c r="B203">
-        <v>67252.772683000003</v>
+        <v>43472.317158999998</v>
       </c>
       <c r="C203">
-        <v>47588.86894</v>
+        <v>-70419.774533000003</v>
       </c>
       <c r="D203">
-        <v>1629.2763110000001</v>
+        <v>1751.2200660000001</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>203</v>
+        <v>29</v>
       </c>
       <c r="B204">
-        <v>67493.248152</v>
+        <v>43295.335779000001</v>
       </c>
       <c r="C204">
-        <v>47778.155313000003</v>
+        <v>-70136.483240000001</v>
       </c>
       <c r="D204">
-        <v>1629.3095599999999</v>
+        <v>1751.220343</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>204</v>
+        <v>165</v>
       </c>
       <c r="B205">
-        <v>66459.058248999994</v>
+        <v>39585.376396</v>
       </c>
       <c r="C205">
-        <v>49090.378942000003</v>
+        <v>-72254.683655999994</v>
       </c>
       <c r="D205">
-        <v>1629.371404</v>
+        <v>1628.1049169999999</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>205</v>
+        <v>164</v>
       </c>
       <c r="B206">
-        <v>66218.352562999993</v>
+        <v>39718.446564999998</v>
       </c>
       <c r="C206">
-        <v>48901.380145000003</v>
+        <v>-72530.282166000005</v>
       </c>
       <c r="D206">
-        <v>1629.380257</v>
+        <v>1628.0704949999999</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="B207">
-        <v>45066.201516000001</v>
+        <v>38212.722506999999</v>
       </c>
       <c r="C207">
-        <v>68710.854882</v>
+        <v>-73256.766138999999</v>
       </c>
       <c r="D207">
-        <v>1629.427825</v>
+        <v>1628.0296820000001</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>207</v>
+        <v>166</v>
       </c>
       <c r="B208">
-        <v>45223.953046000002</v>
+        <v>38079.786076999997</v>
       </c>
       <c r="C208">
-        <v>68973.056509999995</v>
+        <v>-72981.155689000007</v>
       </c>
       <c r="D208">
-        <v>1629.4256069999999</v>
+        <v>1628.009865</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>208</v>
+        <v>157</v>
       </c>
       <c r="B209">
-        <v>45995.269998000003</v>
+        <v>37276.184647000002</v>
       </c>
       <c r="C209">
-        <v>68509.571150000003</v>
+        <v>-73609.074445999999</v>
       </c>
       <c r="D209">
-        <v>1629.42221</v>
+        <v>1628.139574</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>209</v>
+        <v>158</v>
       </c>
       <c r="B210">
-        <v>45837.512692999997</v>
+        <v>37217.113251000002</v>
       </c>
       <c r="C210">
-        <v>68247.345621999993</v>
+        <v>-73635.723209999996</v>
       </c>
       <c r="D210">
-        <v>1629.4140809999999</v>
+        <v>1628.134816</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>210</v>
+        <v>162</v>
       </c>
       <c r="B211">
-        <v>-45223.625820000001</v>
+        <v>36516.985098999998</v>
       </c>
       <c r="C211">
-        <v>-68972.688909000004</v>
+        <v>-73697.874465999994</v>
       </c>
       <c r="D211">
-        <v>1628.5243049999999</v>
+        <v>1628.0910550000001</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>211</v>
+        <v>161</v>
       </c>
       <c r="B212">
-        <v>-45995.459014</v>
+        <v>36636.268090999998</v>
       </c>
       <c r="C212">
-        <v>-68508.894602</v>
+        <v>-73979.697182000004</v>
       </c>
       <c r="D212">
-        <v>1628.5006980000001</v>
+        <v>1628.0651339999999</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>212</v>
+        <v>160</v>
       </c>
       <c r="B213">
-        <v>-45837.370858000002</v>
+        <v>36247.700392999999</v>
       </c>
       <c r="C213">
-        <v>-68246.860858</v>
+        <v>-74144.615888</v>
       </c>
       <c r="D213">
-        <v>1628.4827760000001</v>
+        <v>1628.0841680000001</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>213</v>
+        <v>159</v>
       </c>
       <c r="B214">
-        <v>-45065.781927999997</v>
+        <v>36128.535488000001</v>
       </c>
       <c r="C214">
-        <v>-68710.522498999999</v>
+        <v>-73862.685796000005</v>
       </c>
       <c r="D214">
-        <v>1628.5256119999999</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
-        <v>214</v>
-      </c>
-      <c r="B215">
-        <v>73608.770881999997</v>
-      </c>
-      <c r="C215">
-        <v>37274.857794000003</v>
-      </c>
-      <c r="D215">
-        <v>1629.200585</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
-        <v>215</v>
-      </c>
-      <c r="B216">
-        <v>73635.324869000004</v>
-      </c>
-      <c r="C216">
-        <v>37216.005539999998</v>
-      </c>
-      <c r="D216">
-        <v>1629.1920150000001</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>216</v>
-      </c>
-      <c r="B217">
-        <v>73697.872711000004</v>
-      </c>
-      <c r="C217">
-        <v>36515.557012999998</v>
-      </c>
-      <c r="D217">
-        <v>1629.039628</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>217</v>
-      </c>
-      <c r="B218">
-        <v>73862.664378999994</v>
-      </c>
-      <c r="C218">
-        <v>36127.337134000001</v>
-      </c>
-      <c r="D218">
-        <v>1629.0466329999999</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>218</v>
-      </c>
-      <c r="B219">
-        <v>74144.397203999994</v>
-      </c>
-      <c r="C219">
-        <v>36246.825122000002</v>
-      </c>
-      <c r="D219">
-        <v>1629.0436850000001</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>219</v>
-      </c>
-      <c r="B220">
-        <v>73979.585307000001</v>
-      </c>
-      <c r="C220">
-        <v>36635.028830000003</v>
-      </c>
-      <c r="D220">
-        <v>1629.0476160000001</v>
+        <v>1628.0704330000001</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D214">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>